<commit_message>
Adds columns to export
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -10,7 +10,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Verdana"/>
       <sz val="10"/>
@@ -18,6 +18,11 @@
     <font>
       <name val="Verdana"/>
       <sz val="8"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,8 +39,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -363,6 +369,1413 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
-  <sheetData/>
+  <dimension ref="A1:H87"/>
+  <cols>
+    <col min="1" max="1" width="50.7109375" customWidth="1"/>
+    <col min="2" max="2" width="70.7109375" customWidth="1"/>
+    <col min="3" max="3" width="70.7109375" customWidth="1"/>
+    <col min="4" max="4" width="70.7109375" customWidth="1"/>
+    <col min="5" max="5" width="70.7109375" customWidth="1"/>
+    <col min="6" max="6" width="70.7109375" customWidth="1"/>
+    <col min="7" max="7" width="70.7109375" customWidth="1"/>
+    <col min="8" max="8" width="70.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" customFormat="false">
+      <c r="A1" s="1" t="str">
+        <v>Subject</v>
+      </c>
+      <c r="B1" s="1" t="str">
+        <v>Test Name</v>
+      </c>
+      <c r="C1" s="1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="D1" s="1" t="str">
+        <v>preconditions</v>
+      </c>
+      <c r="E1" s="1" t="str">
+        <v>step_number</v>
+      </c>
+      <c r="F1" s="1" t="str">
+        <v>actions</v>
+      </c>
+      <c r="G1" s="1" t="str">
+        <v>expectedresults</v>
+      </c>
+      <c r="H1" s="1" t="str">
+        <v>Type</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" customFormat="false">
+      <c r="A2" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B2" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="C2" s="0" t="str">
+        <v xml:space="preserve"> 
+</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" customFormat="false">
+      <c r="A3" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B3" s="0" t="str">
+        <v>Configuração de Parâmetros</v>
+      </c>
+      <c r="C3" s="0" t="str">
+        <v>&lt;p&gt; Configurar os parâmetros do sistema.&lt;/p&gt;</v>
+      </c>
+      <c r="D3" s="0" t="str">
+        <v>&lt;p&gt; Ter acesso a alteração de parâmetros.&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" customFormat="false">
+      <c r="A4" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B4" s="0" t="str">
+        <v>Configurações do Sistema</v>
+      </c>
+      <c r="C4" s="0" t="str">
+        <v>&lt;p&gt; Configurar o sistema.&lt;/p&gt;</v>
+      </c>
+      <c r="D4" s="0" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:4" customFormat="false">
+      <c r="A5" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B5" s="0" t="str">
+        <v>Cadastro de Organização</v>
+      </c>
+      <c r="C5" s="0" t="str">
+        <v>&lt;p&gt; Efetuar a configuração das organizações cadastradas no Import ou Export Sys para que possam ser integradas com o RegInt Sys.&lt;/p&gt;</v>
+      </c>
+      <c r="D5" s="0" t="str">
+        <v>&lt;p&gt; Ter Organizações cadastradas no Import ou Export Sys.&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" customFormat="false">
+      <c r="A6" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B6" s="0" t="str">
+        <v>Cadastro de Parceiros</v>
+      </c>
+      <c r="C6" s="0" t="str">
+        <v>&lt;p&gt; Cadastrar parceiros para serem usados na integração com Import e Export Sys.&lt;/p&gt;</v>
+      </c>
+      <c r="D6" s="0" t="str">
+        <v>&lt;p&gt;Ter o CNPJ cadastrado  no parâmetro "NIT" do cadastro de Parâmetros.&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" customFormat="false">
+      <c r="A7" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B7" s="0" t="str">
+        <v>Cadastro de Produtos</v>
+      </c>
+      <c r="C7" s="0" t="str">
+        <v>&lt;p&gt; Configurar os produtos cadastrados com informações de campos extras necessárias para integração do Import/Export com RegInt.&lt;/p&gt;</v>
+      </c>
+      <c r="D7" s="0" t="str">
+        <v>&lt;p&gt; Ter produtos cadastrados nom Import / Export&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" customFormat="false">
+      <c r="A8" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B8" s="0" t="str">
+        <v>Validar a criação do parâmetro CONSUMO_PROPORCIONAL.</v>
+      </c>
+      <c r="C8" s="0" t="str">
+        <v>&lt;p&gt; Validar se o parâmetro CONSUMO_PROPORCIONAL está sendo criado corretamente.&lt;/p&gt;</v>
+      </c>
+      <c r="D8" s="0" t="str">
+        <v>&lt;p&gt; N/A&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" customFormat="false">
+      <c r="A9" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B9" s="0" t="str">
+        <v>Validar a criação do parâmetro DIVERGENCIA_QUANT_CONS_UNIT.</v>
+      </c>
+      <c r="C9" s="0" t="str">
+        <v>&lt;p&gt; Validar se o parâmetro DIVERGENCIA_QUANNT_CONS_UNIT está sendo criado corretamente.&lt;/p&gt;</v>
+      </c>
+      <c r="D9" s="0" t="str">
+        <v>&lt;p&gt; N/A&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" customFormat="false">
+      <c r="A10" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B10" s="0" t="str">
+        <v>Validar combinação de parâmetros.</v>
+      </c>
+      <c r="C10" s="0" t="str">
+        <v>&lt;p&gt;Validar se o sistema está permitindo deixar os parâmetros DIVERGENCIA_QUANT_CONS_UNIT e CONSUMO_PROPORCIONAL ambos com o valor 'S'.&lt;/p&gt;</v>
+      </c>
+      <c r="D10" s="0" t="str">
+        <v>&lt;p&gt;Os parâmetros DIVERGENCIA_QUANT_CONS_UNIT e CONSUMO_PROPORCIONAL devem estar com o valor 'N'.&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" customFormat="false">
+      <c r="A11" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B11" s="0" t="str">
+        <v>Fluxo Básico da Exportação do Tipo 10</v>
+      </c>
+      <c r="C11" s="0" t="str">
+        <v>&lt;p&gt; Executar os testes do documento em anexo.&lt;/p&gt;</v>
+      </c>
+      <c r="D11" s="0" t="str">
+        <v>&lt;p&gt; Ter a base consfigurada para integração Import x Export x RegInt.&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" customFormat="false">
+      <c r="A12" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B12" s="0" t="str">
+        <v>Fluxo Básico da Exportação do Tipo 20</v>
+      </c>
+      <c r="C12" s="0" t="str">
+        <v>&lt;p&gt; Executar os testes do documento em anexo.&lt;/p&gt;</v>
+      </c>
+      <c r="D12" s="0" t="str">
+        <v>&lt;p&gt; Ter a base consfigurada para integração Import x Export x RegInt.&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" customFormat="false">
+      <c r="A13" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B13" s="0" t="str">
+        <v>Fluxo Básico da Exportação do Tipo 30</v>
+      </c>
+      <c r="C13" s="0" t="str">
+        <v>&lt;p&gt; Executar os testes do documento em anexo.&lt;/p&gt;</v>
+      </c>
+      <c r="D13" s="0" t="str">
+        <v>&lt;p&gt; Ter a base consfigurada para integração Import x Export x RegInt.&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" customFormat="false">
+      <c r="A14" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B14" s="0" t="str">
+        <v>Fluxo Básico da Exportação do Tipo 40</v>
+      </c>
+      <c r="C14" s="0" t="str">
+        <v>&lt;p&gt; Executar os testes do documento em anexo.&lt;/p&gt;</v>
+      </c>
+      <c r="D14" s="0" t="str">
+        <v>&lt;p&gt; Ter a base consfigurada para integração Import x Export x RegInt.&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" customFormat="false">
+      <c r="A15" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B15" s="0" t="str">
+        <v>Fluxo Básico da Nacionalização e Estorno</v>
+      </c>
+      <c r="C15" s="0" t="str">
+        <v>&lt;p&gt; Testes de Nacionalização e Estorno do Processo de Nacionalização.&lt;/p&gt;</v>
+      </c>
+      <c r="D15" s="0" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:4" customFormat="false">
+      <c r="A16" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B16" s="0" t="str">
+        <v>Fluxo Básico da Exportação para Regime Automotivo</v>
+      </c>
+      <c r="C16" s="0" t="str">
+        <v>&lt;p&gt;Fluxo de testes de regime automotivo&lt;/p&gt;</v>
+      </c>
+      <c r="D16" s="0" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:4" customFormat="false">
+      <c r="A17" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B17" s="0" t="str">
+        <v>Fluxo Básico da Exportação com Remito de Entrada</v>
+      </c>
+      <c r="C17" s="0" t="str">
+        <v>&lt;p&gt; Executar o fluxo completo com Remito de Entrada.&lt;/p&gt;</v>
+      </c>
+      <c r="D17" s="0" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:4" customFormat="false">
+      <c r="A18" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B18" s="0" t="str">
+        <v>Fluxo Básico da Reposição de Estoque - Exportação Direta</v>
+      </c>
+      <c r="C18" s="0" t="str">
+        <v>&lt;p&gt; Fluxo completo para Reposição de Estoque de Exportações diretas.&lt;/p&gt;</v>
+      </c>
+      <c r="D18" s="0" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:4" customFormat="false">
+      <c r="A19" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B19" s="0" t="str">
+        <v>Fluxo Básico da Reposição de Estoque - Exportação Indireta</v>
+      </c>
+      <c r="C19" s="0" t="str">
+        <v>&lt;p&gt; Fluxo completo para Reposição de Estoque de Exportações indiretas.&lt;/p&gt;</v>
+      </c>
+      <c r="D19" s="0" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:4" customFormat="false">
+      <c r="A20" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B20" s="0" t="str">
+        <v xml:space="preserve">Verificar funcionalidades disponíveis para o módulo </v>
+      </c>
+      <c r="C20" s="0" t="str">
+        <v/>
+      </c>
+      <c r="D20" s="0" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:3" customFormat="false">
+      <c r="A21" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B21" s="0" t="str">
+        <v>Cadastros e Configurações Iniciais</v>
+      </c>
+      <c r="C21" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt; Suíte para casdastros e configurações básicas do sistema.&lt;/p&gt;
+&lt;p&gt;Configurações para integração com Import e Export.&lt;/p&gt; 
+</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" customFormat="false">
+      <c r="A22" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B22" s="0" t="str">
+        <v>Fluxos</v>
+      </c>
+      <c r="C22" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt; Fluxo dos tipos 10,20,30 e 40&lt;/p&gt; 
+</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" customFormat="false">
+      <c r="A23" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B23" s="0" t="str">
+        <v>Realizar Sugestão de Exportação Normal com baixa com CTIT 001</v>
+      </c>
+      <c r="C23" s="0" t="str">
+        <v>&lt;p&gt;Realizar uma sugestão de exportação normal (Tipo 10) para um item presente em um CTIT, com consumo da baixa pela estrutura do CTIT, onde o CTIT possui em seu preenchimento o número de CTIT preenchido, o número de Protocolo e o número de ITP. Após a realização da sugestão, verificar que a flag "C_CONSUMO_REP_EST" na tabela "RI_SUGESTAO_EXPO_ITEM" recebe o valor "S" pois no momento da baixa houve consumo de Remito de Parceiro com tipo "R". Verificar que a flag "C_CONSUMO_REP_EST_EMP" na tabela "RI_SUGESTAO_EXPO_ITEM" recebe o valor "N", pois não houve consumo de DI's do tipo IA ou IC da própria empresa, sendo o consumo de DI's em sua totalidade de DI's do tipo IT (Importação Temporal).&lt;/p&gt;</v>
+      </c>
+      <c r="D23" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;1 - Usuário do Export Sys com permissão para cadastro de processos de exportação;&lt;br /&gt;
+2 - Usuário do IT Sys com permissão para Consulta de DI's, consulta de documentos de entrada de parceiros e consulta de pendências de baixa;&lt;br /&gt;
+3 - CTIT cadastrado e ativo com o número de CTIT, o número de Protocolo e o número de ITP. O CTIT deve realizar o consumo pela estrutura do CTIT;&lt;br /&gt;
+4 - Para o CTIT informado acima, o mesmo deve possuir em seu cadastro, um produto acabado "PN A" e em sua estrutura os insumos "PN B", " PN C" e "PN D";&lt;br /&gt;
+5 - Estrutura de produto para o produto acabado "PN A" mais recente que a utilizada na criação do CTIT citado na pré-condição de número 4 e que em sua estrutura possua os seguintes insumos: "PN B", "PN E" e "PN G";&lt;br /&gt;
+6 - DI do tipo IA para o insumo "PN E" com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;br /&gt;
+7 - DI do tipo IC para o insumo "PN G"  com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;br /&gt;
+8 - DI do tipo IT para o insumo "PN B"  com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;br /&gt;
+9 - Remito de parceiro do tipo "R" para o insumo "PN D" com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" customFormat="false">
+      <c r="A24" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B24" s="0" t="str">
+        <v>Realizar Sugestão de Exportação Normal com baixa com CTIT 002</v>
+      </c>
+      <c r="C24" s="0" t="str">
+        <v>&lt;p&gt;Realizar uma sugestão de exportação normal (Tipo 10) para um item presente em um CTIT, com consumo da baixa pela estrutura do CTIT, onde o CTIT possui em seu preenchimento somente o número de ITP. Após a realização da sugestão, verificar que a flag "C_CONSUMO_REP_EST" na tabela "RI_SUGESTAO_EXPO_ITEM" recebe o valor "N" pois no momento da baixa não houve consumo de Remito de Parceiro com tipo "R". Verificar que a flag "C_CONSUMO_REP_EST_EMP" na tabela "RI_SUGESTAO_EXPO_ITEM" recebe o valor "S", pois houve consumo de DI's do tipo IA ou IC da própria empresa.&lt;/p&gt;</v>
+      </c>
+      <c r="D24" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;1 - Usuário do Export Sys com permissão para cadastro de processos de exportação;&lt;br /&gt;
+2 - Usuário do IT Sys com permissão para Consulta de DI's, consulta de documentos de entrada de parceiros e consulta de pendências de baixa;&lt;br /&gt;
+3 - CTIT cadastrado e ativo com somente com o número de ITP preenchido. O CTIT deve realizar o consumo pela estrutura do CTIT;&lt;br /&gt;
+4 - Para o CTIT informado acima, o mesmo deve possuir em seu cadastro, um produto acabado "PN A" e em sua estrutura os insumos "PN B", " PN C" e "PN D";&lt;br /&gt;
+5 - Estrutura de produto para o produto acabado "PN A" mais recente que a utilizada na criação do CTIT citado na pré-condição de número 4 e que em sua estrutura possua os seguintes insumos: "PN B", "PN E" e "PN G";&lt;br /&gt;
+6 - DI do tipo IA para o insumo "PN E" com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;br /&gt;
+7 - DI do tipo IC para o insumo "PN B"  com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;br /&gt;
+8 - DI do tipo IC para o insumo "PN D"  com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;br /&gt;
+9 - Remito de parceiro do tipo "R" para o insumo "PN E" com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" customFormat="false">
+      <c r="A25" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B25" s="0" t="str">
+        <v>Realizar Sugestão de Exportação Normal com baixa com CTIT 003</v>
+      </c>
+      <c r="C25" s="0" t="str">
+        <v>&lt;p&gt;Realizar uma sugestão de exportação normal (Tipo 10) para um item presente em um CTIT, com consumo da baixa pela estrutura do produto acabado, onde o CTIT possui em seu preenchimento o número de CTIT preenchido, o número de Protocolo e o número de ITP. Após a realização da sugestão, verificar que a flag "C_CONSUMO_REP_EST" na tabela "RI_SUGESTAO_EXPO_ITEM" recebe o valor "S" pois no momento da baixa houve consumo de Remito de Parceiro com tipo "R". Verificar que a flag "C_CONSUMO_REP_EST_EMP" na tabela "RI_SUGESTAO_EXPO_ITEM" recebe o valor "S", pois houve consumo de DI's do tipo IA ou IC da própria empresa, porém agora existem subitens de DI's com número atuação de reposição de estoque para consumo no processamento da baixa.&lt;/p&gt;</v>
+      </c>
+      <c r="D25" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;1 - Usuário do Export Sys com permissão para cadastro de processos de exportação;&lt;br /&gt;
+2 - Usuário do IT Sys com permissão para Consulta de DI's, consulta de documentos de entrada de parceiros e consulta de pendências de baixa;&lt;br /&gt;
+3 - CTIT cadastrado e ativo com o número de CTIT, número de Protocolo e o número de ITP. O CTIT não deve realizar o consumo de pela estrutura do CTIT;&lt;br /&gt;
+4 - Para o CTIT informado acima, o mesmo deve possuir em seu cadastro, um produto acabado "PN A" e em sua estrutura os insumos "PN B", " PN C" e "PN D";&lt;br /&gt;
+5 - Estrutura de produto para o produto acabado "PN A" mais recente que a utilizada na criação do CTIT citado na pré-condição de número 4 e que em sua estrutura possua os seguintes insumos: "PN B", "PN E" e "PN G";&lt;br /&gt;
+6 - DI do tipo IC para o insumo "PN G" com saldo para consumo, número de atuação de reposição de estoque preenchido e data de registro dentro do período para consumo para baixa;&lt;br /&gt;
+7 - DI do tipo IA com dois subitens, sendo um para o insumo "PN B" com saldo para consumo, número de atuação para reposição de estoque e data de registro dentro do período para consumo para baixa e um segundo subitem para o insumo "PN G" com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;br /&gt;
+8 - DI do tipo IT para o insumo "PN E" com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;br /&gt;
+9 - Remito de parceiro do tipo "R" para o insumo "PN E" com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" customFormat="false">
+      <c r="A26" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B26" s="0" t="str">
+        <v>Realizar Sugestão de Exportação Normal com baixa com CTIT 004</v>
+      </c>
+      <c r="C26" s="0" t="str">
+        <v>&lt;p&gt;Realizar uma sugestão de exportação normal (Tipo 10) para um item presente em um CTIT, com consumo da baixa pela OP do produto acabado, onde o CTIT possui em seu preenchimento o número de Protocolo e o número de ITP. Após a realização da sugestão, verificar que a flag "C_CONSUMO_REP_EST" na tabela "RI_SUGESTAO_EXPO_ITEM" recebe o valor "N" pois no momento da baixa não houve consumo de Remito de Parceiro com tipo "R". Verificar que a flag "C_CONSUMO_REP_EST_EMP" na tabela "RI_SUGESTAO_EXPO_ITEM" recebe o valor "S", pois houve consumo de DI's do tipo IA ou IC da própria empresa.&lt;/p&gt;</v>
+      </c>
+      <c r="D26" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;1 - Usuário do Export Sys com permissão para cadastro de processos de exportação;&lt;br /&gt;
+2 - Usuário do IT Sys com permissão para Consulta de DI's, consulta de documentos de entrada de parceiros e consulta de pendências de baixa;&lt;br /&gt;
+3 - CTIT cadastrado com o número de Protocolo e o número de ITP. O CTIT não deve realizar o consumo de pela estrutura do CTIT;;&lt;br /&gt;
+4 - Para o CTIT informado acima, o mesmo deve possuir em seu cadastro, um produto acabado "PN A" e em sua estrutura os insumos "PN B", " PN C" e "PN D";&lt;br /&gt;
+5 - Estrutura de produto para o produto acabado "PN A" mais recente que a utilizada na criação do CTIT citado na pré-condição de número 4 e que em sua estrutura possua os seguintes insumos: "PN B", "PN E" e "PN G";&lt;br /&gt;
+6 - DI do tipo IA para o insumo "PN G" com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;br /&gt;
+7 - DI do tipo IA para o insumo "PN B" com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;br /&gt;
+8 - DI do tipo IC para o insumo "PN D" com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;br /&gt;
+9 - Remito de parceiro do tipo "R" para o insumo "PN C" com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" customFormat="false">
+      <c r="A27" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B27" s="0" t="str">
+        <v>Realizar Sugestão de Exportação Normal com baixa com CTIT 005</v>
+      </c>
+      <c r="C27" s="0" t="str">
+        <v>&lt;p&gt;Realizar uma sugestão de exportação normal (Tipo 10) de modo que na sugestão de exportação possua dois itens de modo que para cada item de sugestão seja retornado um CTIT diferente. Em um dos CTIT's o mesmo deve possuir em seu preenchimento o número de CTIT, número de protocolo e número de ITP. No outro CTIT, deve possuir apenas o número de ITP. Após o processamento da baixa, verficar as flags "C_CONSUMO_REP_EST_EMP" e "C_CONSUMO_REP_EST" na tabela "RI_SUGESTAO_EXPO_ITEM", ambas receberão o valor "S", porem em um item de sugestão terá consumo de DI's do tipo IA e IC e para o outro item consumo apenas de Remito de Parceiro do tipo "R".&lt;/p&gt;</v>
+      </c>
+      <c r="D27" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;1 - Usuário do Export Sys com permissão para cadastro de processos de exportação;&lt;br /&gt;
+2 - Usuário do IT Sys com permissão para Consulta de DI's, consulta de documentos de entrada de parceiros e consulta de pendências de baixa;&lt;br /&gt;
+3 - CTIT "CTIT_1" cadastrado com número de CTIT, número de Protocolo e o número de ITP. O CTIT deve realizar o consumo de pela estrutura do CTIT;&lt;br /&gt;
+4 - CTIT "CTIT_2" cadastrado somente com número de ITP. O CTIT não deve realizar o consumo de pela estrutura do CTIT;&lt;br /&gt;
+5 - Para o CTIT "CTIT_1", o mesmo deve possuir em seu cadastro, um produto acabado "PN A" e em sua estrutura os insumos "PN B", " PN C" e "PN D";&lt;br /&gt;
+6 - Para o CTIT "CTIT_2", o mesmo deve possuir em seu cadastro, um produto acabado "PN X" e em sua estrutura os insumos "PN Y", " PN Z" e "PN E";&lt;br /&gt;
+7 - Estrutura de produto para o produto acabado "PN A" mais recente que a utilizada na criação do CTIT citado na pré-condição de número 5 e que em sua estrutura possua os seguintes insumos: "PN B", "PN E" e "PN G";&lt;br /&gt;
+8 - Estrutura de produto para o produto acabado "PN X" mais recente que a utilizada na criação do CTIT citado na pré-condição de número 6 e que em sua estrutura possua os seguintes insumos: "PN Y", "PN Z" e "PN D";&lt;br /&gt;
+9 - DI do tipo IA para o insumo "PN G" com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;br /&gt;
+10 - DI do tipo IT para o insumo "PN B"  com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;br /&gt;
+11 - DI do tipo IT para o insumo "PN D"  com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;br /&gt;
+12 - Remito de parceiro do tipo "R" para o insumo "PN D" com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;br /&gt;
+13 - DI do tipo IA para o insumo "PN Y" com saldo para consumo, número de atuação para reposição de estoque preenchido e data de registro dentro do período para consumo para baixa;&lt;br /&gt;
+14 - DI do tipo IC para o insumo "PN Z"  com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" customFormat="false">
+      <c r="A28" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B28" s="0" t="str">
+        <v>Realizar Sugestão de Exportação Normal com baixa com CTIT 006</v>
+      </c>
+      <c r="C28" s="0" t="str">
+        <v>&lt;p&gt;Realizar uma sugestão de exportação normal (Tipo 10) para um item presente em um CTIT, com consumo da baixa pela OP do produto acabado, onde o CTIT possui em seu preenchimento o número de Protocolo e o número de ITP. Após a realização da sugestão, verificar que a flag "C_CONSUMO_REP_EST" na tabela "RI_SUGESTAO_EXPO_ITEM" recebe o valor "S" pois no momento da baixa não houve consumo de Remito de Parceiro com tipo "R", porém a baixa foi realizada para um item equivalente. Verificar que a flag "C_CONSUMO_REP_EST_EMP" na tabela "RI_SUGESTAO_EXPO_ITEM" recebe o valor "S", pois houve consumo de DI's do tipo IA ou IC da própria empresa para um item equivalente.&lt;/p&gt;</v>
+      </c>
+      <c r="D28" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;1 - Usuário do Export Sys com permissão para cadastro de processos de exportação;&lt;br /&gt;
+2 - Usuário do IT Sys com permissão para Consulta de DI's, consulta de documentos de entrada de parceiros e consulta de pendências de baixa;&lt;br /&gt;
+3 - CTIT cadastrado com o número de Protocolo e o número de ITP;&lt;br /&gt;
+4 - Para o CTIT informado acima, o mesmo deve possuir em seu cadastro, um produto acabado "PN A" e em sua estrutura os insumos "PN B", " PN C" e "PN D";&lt;br /&gt;
+5 - Estrutura de produto para o produto acabado "PN A" mais recente que a utilizada na criação do CTIT citado na pré-condição de número 4 e que em sua estrutura possua os seguintes insumos: "PN B", "PN E" e "PN G";&lt;br /&gt;
+6 - Grupo de equivência contendo em um mesmo grupo os seguintes insumos: "PN B" e "PN F";&lt;br /&gt;
+7 - Grupo de equivência contendo em um mesmo grupo os seguintes insumos: "PN G" e "PN K"&lt;br /&gt;
+8 - DI do tipo IA para o insumo "PN C" com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;br /&gt;
+9 - DI do tipo IA para o insumo "PN F"  com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;br /&gt;
+10 - DI do tipo IC para o insumo "PN K"  com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;br /&gt;
+11 - Remito de parceiro do tipo "R" para o insumo "PN K" com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" customFormat="false">
+      <c r="A29" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B29" s="0" t="str">
+        <v>Realizar Sugestão de Exportação Normal com baixa com CTIT 007</v>
+      </c>
+      <c r="C29" s="0" t="str">
+        <v>&lt;p&gt;Realizar uma sugestão de exportação normal (Tipo 10) de modo que na sugestão de exportação possua dois itens de modo que para cada item de sugestão seja retornado um CTIT diferente. Em um dos CTIT's o mesmo deve possuir em seu preenchimento o número de CTIT, número de protocolo e número de ITP. No outro CTIT, deve possuir apenas o número de ITP. Para este caso, no processamento da baixa os dois itens devem consumuir um mesmo documento de entrada. Após o processamento da baixa, verficar as flags "C_CONSUMO_REP_EST_EMP" e "C_CONSUMO_REP_EST" na tabela "RI_SUGESTAO_EXPO_ITEM" para cada item de sugestão.&lt;/p&gt;</v>
+      </c>
+      <c r="D29" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;1 - Usuário do Export Sys com permissão para cadastro de processos de exportação;&lt;br /&gt;
+2 - Usuário do IT Sys com permissão para Consulta de DI's, consulta de documentos de entrada de parceiros e consulta de pendências de baixa;&lt;br /&gt;
+3 - CTIT "CTIT_1" cadastrado com número de CTIT, número de Protocolo e o número de ITP. O CTIT deve realizar o consumo de pela estrutura do CTIT;&lt;br /&gt;
+4 - CTIT "CTIT_2" cadastrado somente com número de ITP. O CTIT deve realizar o consumo de pela estrutura do produto acabado;&lt;br /&gt;
+5 - Para o CTIT "CTIT_1", o mesmo deve possuir em seu cadastro, um produto acabado "PN A" e em sua estrutura os insumos "PN B", " PN C" e "PN D";&lt;br /&gt;
+6 - Para o CTIT "CTIT_2", o mesmo deve possuir em seu cadastro, um produto acabado "PN X" e em sua estrutura os insumos "PN Y", " PN Z" e "PN E";&lt;br /&gt;
+7 - Estrutura de produto para o produto acabado "PN A" mais recente que a utilizada na criação do CTIT citado na pré-condição de número 5 e que em sua estrutura possua os seguintes insumos: "PN B", "PN E" e "PN G";&lt;br /&gt;
+8 - Estrutura de produto para o produto acabado "PN X" mais recente que a utilizada na criação do CTIT citado na pré-condição de número 6 e que em sua estrutura possua os seguintes insumos: "PN Y", "PN Z" e "PN D";&lt;br /&gt;
+9 - DI do tipo IA para o insumo "PN G" com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;br /&gt;
+10 - DI do tipo IT para o insumo "PN B"  com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;br /&gt;
+11 - DI do tipo IC para o insumo "PN D"  com saldo para consumo e data de registro dentro do período para consumo para baixa (Obs.: Para essa DI, ter uma grande quantidade de saldo de modo que seja consumida pelos dois itens de sugestão de exportação);&lt;br /&gt;
+12 - Remito de parceiro do tipo "R" para o insumo "PN D" com data de emissão anterior à data de registro da DI citada na pré-condição de número 11, com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;br /&gt;
+13 - DI do tipo IA para o insumo "PN Y" com saldo para consumo, número de atuação para reposição de estoque preenchido e data de registro dentro do período para consumo para baixa;&lt;br /&gt;
+14 - DI do tipo IC para o insumo "PN Z"  com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" customFormat="false">
+      <c r="A30" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B30" s="0" t="str">
+        <v>Realizar Exportação tipo 20 para Reexportação</v>
+      </c>
+      <c r="C30" s="0" t="str">
+        <v>&lt;p&gt;Realizar uma reexportação (tipo 20) de modo que no processamento da baixa seja consumido uma DI do tipo ITS de modo que o produto informado no item da sugestão de exportação seja o produto informado na DI do tipo ITS (Importação Temporal Sem Transformação). Após a entrada e processamento da sugestão, verficar as flags "C_CONSUMO_REP_EST_EMP" e "C_CONSUMO_REP_EST" na tabela "RI_SUGESTAO_EXPO_ITEM" para cada item de sugestão, onde ambas receberão sempre o valor "N".&lt;/p&gt;</v>
+      </c>
+      <c r="D30" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;1 - Usuário do Export Sys com permissão para cadastro de processos de exportação;&lt;br /&gt;
+2 - Usuário do IT Sys com permissão para Consulta de DI's, consulta de documentos de entrada de parceiros e consulta de pendências de baixa;&lt;br /&gt;
+3 - DI do tipo ITS  para o produto "PN A" com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;br /&gt;
+4 - DI do tipo IA  para o produto "PN A" com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;br /&gt;
+5 - DI do tipo IC para o produto "PN A" com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" customFormat="false">
+      <c r="A31" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B31" s="0" t="str">
+        <v>Realizar Sugestão de Exportação Normal com Baixa Direta</v>
+      </c>
+      <c r="C31" s="0" t="str">
+        <v>&lt;p&gt;Realizar uma sugestão de exportação normal (Tipo 10) para um item que não possui um CTIT cadastrado no sistema e nem mesmo uma Estrutura de produto. Sendo o produto a exportar o mesmo presente nos documentos de entrada para baixa. Após a entrada e processamento da sugestão, verficar as flags "C_CONSUMO_REP_EST_EMP" e "C_CONSUMO_REP_EST" na tabela "RI_SUGESTAO_EXPO_ITEM" para cada item de sugestão, onde ambas receberão sempre o valor "N".&lt;/p&gt;</v>
+      </c>
+      <c r="D31" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;1 - Usuário do Export Sys com permissão para cadastro de processos de exportação;&lt;br /&gt;
+2 - Usuário do IT Sys com permissão para Consulta de DI's, consulta de documentos de entrada de parceiros e consulta de pendências de baixa;&lt;br /&gt;
+3 - O produto "PN A" não deve possuir nenhuma estrutura de produto cadastrada e consquentemente nenhum CTIT;&lt;br /&gt;
+4 - DI do tipo ITS  para o produto "PN A" com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;br /&gt;
+5 - DI do tipo IA  para o produto "PN A" com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;br /&gt;
+6 - DI do tipo IC para o produto "PN A" com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;br /&gt;
+7 - DI do tipo IC para o produto "PN A" com saldo para consumo, número de atuação de reposição de estoque preenchido  e data de registro dentro do período para consumo para baixa;&lt;br /&gt;
+8 - Remito de parceiro do tipo "R" para o produto "PN A" com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" customFormat="false">
+      <c r="A32" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B32" s="0" t="str">
+        <v>Realizar Sugestão de Exportação Normal com baixa sem CTIT 001</v>
+      </c>
+      <c r="C32" s="0" t="str">
+        <v>&lt;p&gt;Realizar uma sugestão de exportação normal (Tipo 10) para um item sem CTIT . Após a realização da sugestão, verificar que a flag "C_CONSUMO_REP_EST" na tabela "RI_SUGESTAO_EXPO_ITEM" recebe o valor "S" pois no momento da baixa houve consumo de Remito de Parceiro com tipo "R". Verificar que a flag "C_CONSUMO_REP_EST_EMP" na tabela "RI_SUGESTAO_EXPO_ITEM" recebe o valor "N".&lt;/p&gt;</v>
+      </c>
+      <c r="D32" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;1 - Usuário do Export Sys com permissão para cadastro de processos de exportação;&lt;br /&gt;
+2 - Usuário do IT Sys com permissão para Consulta de DI's, consulta de documentos de entrada de parceiros e consulta de pendências de baixa;&lt;br /&gt;
+3 - Produto acabado "PN A" e em sua estrutura os insumos "PN B", " PN C" e "PN D";&lt;br /&gt;
+4 - DI do tipo IA para o insumo "PN C" com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;br /&gt;
+5 - DI do tipo IC para o insumo "PN D"  com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;br /&gt;
+6 - DI do tipo IC para o insumo "PN D"  com saldo para consumo, número de atuação de reposição de estoque preenchido e data de registro dentro do período para consumo para baixa;&lt;br /&gt;
+7 - DI do tipo IT para o insumo "PN B"  com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;br /&gt;
+8 - Remito de parceiro do tipo "R" para o insumo "PN D" com saldo para consumo e data de registro dentro do período para consumo para baixa;&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" customFormat="false">
+      <c r="A33" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B33" s="0" t="str">
+        <v>Emitir XML Softway2Broker para processo de exportação com consumo de Remito tipo R e DI's IT</v>
+      </c>
+      <c r="C33" s="0" t="str">
+        <v>&lt;p&gt;Emitir um arquivo XML de envio de informação de processo de exportação para despachante (ExpoRepoStock) para um processo de exportação com baixa realizada no RegInt (Exportação tipo 10 com CTIT) e somente consumo de DI to tipo IT (Importação Temporal) e Remitos de Parceiro do tipo "R" o que sinaliza que o item possui consumo de itens de reposição de estoque de parceiros". Ao emitir o arquivo XML, verificar que as tags de reposição de estoque recebem os seguintes valores: "ItemExpoRepoStock" recebe o valor "S" e "ItemExpoRepoStockCompany" recebe o valor "N".&lt;/p&gt;</v>
+      </c>
+      <c r="D33" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;1 - Processo de Exportação no Export Sys pronto para execução  da interface de saída "Softway2Broker" do Export Sys;&lt;br /&gt;
+2 - Usuário do In-Out com permissão para execução da interface de saída "Softway2Broker" do Export Sys;&lt;br /&gt;
+3 - O processo de exportação (Exportação tipo 10 com CTIT)﻿ descrito na pré-condição número 1 deve possuir consumo apenas de DI's do tipo IT e Remitos de Parceiro do Tipo R.&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" customFormat="false">
+      <c r="A34" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B34" s="0" t="str">
+        <v>Emitir XML Softway2Broker para processo de exportação com consumo de DI's IA</v>
+      </c>
+      <c r="C34" s="0" t="str">
+        <v>&lt;p&gt;Emitir um arquivo XML de envio de informação de processo de exportação para despachante (ExpoRepoStock) para um processo de exportação com baixa realizada no RegInt﻿ (Exportação tipo 10 com CTIT)&lt;a id="fck_paste_padding"&gt;﻿&lt;/a&gt; e somente consumo de DI's to tipo IA, o que sinaliza que a declaração de exportação gerada por esse processo estará apta ao pedido de reposição de estoque. Ao emitir o arquivo XML, verificar que as tags de reposição de estoque recebem os seguintes valores: "ItemExpoRepoStock" recebe o valor "N" e "ItemExpoRepoStockCompany" recebe o valor "S".&lt;/p&gt;</v>
+      </c>
+      <c r="D34" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;1 - Processo de Exportação no Export Sys pronto para execução  da interface de saída "Softway2Broker" do Export Sys;&lt;br /&gt;
+2 - Usuário do In-Out com permissão para execução da interface de saída "Softway2Broker" do Export Sys;&lt;br /&gt;
+3 - O processo de exportação﻿ (Exportação tipo 10 com CTIT)﻿&lt;a id="fck_paste_padding"&gt;﻿&lt;/a&gt; descrito na pré-condição número 1 deve possuir consumo apenas de DI's do tipo IA.&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" customFormat="false">
+      <c r="A35" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B35" s="0" t="str">
+        <v>Emitir XML Softway2Broker para processo de exportação com consumo de DI's IC</v>
+      </c>
+      <c r="C35" s="0" t="str">
+        <v>&lt;p&gt;Emitir um arquivo XML de envio de informação de processo de exportação para despachante (ExpoRepoStock) para um processo de exportação com baixa realizada no RegInt﻿ (Exportação tipo 10 com CTIT)&lt;a id="fck_paste_padding"&gt;﻿&lt;/a&gt; e somente consumo de DI's to tipo IC, o que sinaliza que a declaração de exportação gerada por esse processo estará apta ao pedido de reposição de estoque. Ao emitir o arquivo XML, verificar que as tags de reposição de estoque recebem os seguintes valores: "ItemExpoRepoStock" recebe o valor "N" e "ItemExpoRepoStockCompany" recebe o valor "S".&lt;/p&gt;</v>
+      </c>
+      <c r="D35" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;1 - Processo de Exportação no Export Sys pronto para execução  da interface de saída "Softway2Broker" do Export Sys;&lt;br /&gt;
+2 - Usuário do In-Out com permissão para execução da interface de saída "Softway2Broker" do Export Sys;&lt;br /&gt;
+3 - O processo de exportação﻿ (Exportação tipo 10 com CTIT)﻿&lt;a id="fck_paste_padding"&gt;﻿&lt;/a&gt; descrito na pré-condição número 1 deve possuir consumo apenas de DI's do tipo IC com número de atuação de reposição de estoque.&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" customFormat="false">
+      <c r="A36" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B36" s="0" t="str">
+        <v>Emitir XML Softway2Broker para processo de exportação com consumo de DI's IC e Remito do tipo R</v>
+      </c>
+      <c r="C36" s="0" t="str">
+        <v>&lt;p&gt;Emitir um arquivo XML de envio de informação de processo de exportação para despachante (ExpoRepoStock) para um processo de exportação com baixa realizada no RegInt﻿ (Exportação tipo 10 com CTIT)&lt;a id="fck_paste_padding"&gt;﻿&lt;/a&gt; e consumo de DI's to tipo IC, o que sinaliza que a declaração de exportação gerada por esse processo estará apta ao pedido de reposição de estoque.  Remitos de Parceiro do tipo "R" o que sinaliza que o item possui consumo de itens de reposição de estoque de parceiros". Ao emitir o arquivo XML, verificar que as tags de reposição de estoque recebem os seguintes valores: "ItemExpoRepoStock" recebe o valor "S" e "ItemExpoRepoStockCompany" recebe o valor "S".&lt;/p&gt;</v>
+      </c>
+      <c r="D36" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;1 - Processo de Exportação no Export Sys pronto para execução  da interface de saída "Softway2Broker" do Export Sys;&lt;br /&gt;
+2 - Usuário do In-Out com permissão para execução da interface de saída "Softway2Broker" do Export Sys;&lt;br /&gt;
+3 - O processo de exportação﻿ (Exportação tipo 10 com CTIT)﻿&lt;a id="fck_paste_padding"&gt;﻿&lt;/a&gt; descrito na pré-condição número 1 deve possuir consumo apenas de DI's do tipo IC e Remitos de Parceiro do Tipo R.&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" customFormat="false">
+      <c r="A37" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B37" s="0" t="str">
+        <v>Emitir XML Softway2Broker para processo de exportação com consumo de DI's IT</v>
+      </c>
+      <c r="C37" s="0" t="str">
+        <v>&lt;p&gt;Emitir um arquivo XML de envio de informação de processo de exportação para despachante (ExpoRepoStock) para um processo de exportação com baixa realizada no RegInt﻿ (Exportação tipo 10 com CTIT)&lt;a id="fck_paste_padding"&gt;﻿&lt;/a&gt; e somente consumo de DI to tipo IT (Importação Temporal). Ao emitir o arquivo XML, verificar que as tags de reposição de estoque recebem os seguintes valores: "ItemExpoRepoStock" recebe o valor "N" e "ItemExpoRepoStockCompany" recebe o valor "N".&lt;/p&gt;</v>
+      </c>
+      <c r="D37" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;1 - Processo de Exportação no Export Sys pronto para execução  da interface de saída "Softway2Broker" do Export Sys;&lt;br /&gt;
+2 - Usuário do In-Out com permissão para execução da interface de saída "Softway2Broker" do Export Sys;&lt;br /&gt;
+3 - O processo de exportação﻿ (Exportação tipo 10 com CTIT)﻿&lt;a id="fck_paste_padding"&gt;﻿&lt;/a&gt; descrito na pré-condição número 1 deve possuir consumo apenas de DI's do tipo IT.&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" customFormat="false">
+      <c r="A38" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B38" s="0" t="str">
+        <v>Receber DE XML via interface Broker2Softway para processo de exportação com consumo de DI's IT</v>
+      </c>
+      <c r="C38" s="0" t="str">
+        <v>&lt;p&gt;Receber uma declaração de exportação via interface XML Broker2Softway de modo que o processo de exportação cadastrado possua consumo somente de DI's do tipo IT, e consequentemente as flags "CONSUMO_REP_EST" e "CONSUMO_REP_EST_EMP" possuem o valor "N". A Declaração de exportação deve possuir em seu conteúdo as flags "declarationItemExpoRepoStock" e "declarationItemExpoRepoStockCompany" preenchidas com o valor "N".&lt;/p&gt;</v>
+      </c>
+      <c r="D38" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;1 - Processo de exportação cadastrado (Exportação tipo 10 com CTIT)﻿ e com consumo apenas de DI's do tipo IT;&lt;br /&gt;
+2 - Arquivo XML contendo informações de Declaração de Exportação para o processo descrito na pré-condição de número 1 com as tags "declarationItemExpoRepoStock" e "declarationItemExpoRepoStockCompany" preenchidas com o valor "N";&lt;br /&gt;
+3 - Usuário do In-Out com permissão para execução da interface de entrada "Broker2Softway" do Export Sys;&lt;br /&gt;
+4 - Usuário do Export Sys com permissão para consulta de Declaração de Exportação;&lt;br /&gt;
+5 - Usuário do IT Sys com permissão para consulta de Declaração de Exportação.&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" customFormat="false">
+      <c r="A39" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B39" s="0" t="str">
+        <v>Receber DE XML via interface Broker2Softway para processo de exportação com consumo de DI's IA</v>
+      </c>
+      <c r="C39" s="0" t="str">
+        <v>&lt;p&gt;Receber uma declaração de exportação via interface XML Broker2Softway de modo que o processo de exportação cadastrado possua consumo somente de DI's do tipo IA, e consquentemente as flags "CONSUMO_REP_EST" possui o valor "N" e "CONSUMO_REP_EST_EMP" possui o valor "S". A Declaração de exportação deve possuir em seu conteúdo as flags "declarationItemExpoRepoStock" preenchida com o valor "N" e "declarationItemExpoRepoStockCompany" preenchida com o valor "S"&lt;/p&gt;</v>
+      </c>
+      <c r="D39" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;1 - Processo de exportação cadastrado (Exportação tipo 10 com CTIT)﻿ e com consumo apenas de DI's do tipo IA;&lt;br /&gt;
+2 - Arquivo XML contendo informações de Declaração de Exportação para o processo descrito na pré-condição de número 1 com as tags "declarationItemExpoRepoStock" preenchida com o valor "N"; e "declarationItemExpoRepoStockCompany" preenchida com o valor "S";&lt;br /&gt;
+3 - Usuário do In-Out com permissão para execução da interface de entrada "Broker2Softway" do Export Sys;&lt;br /&gt;
+4 - Usuário do Export Sys com permissão para consulta de Declaração de Exportação;&lt;br /&gt;
+5 - Usuário do IT Sys com permissão para consulta de Declaração de Exportação&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" customFormat="false">
+      <c r="A40" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B40" s="0" t="str">
+        <v>Receber DE XML via interface B2S para processo de exportação com consumo de DI's IC e Remitos R</v>
+      </c>
+      <c r="C40" s="0" t="str">
+        <v>&lt;p&gt;Receber uma declaração de exportação via interface XML Broker2Softway de modo que o processo de exportação cadastrado possua consumo de DI's do tipo IC e Remitos de Parceiro com motivo "R", e consequentemente a flag "CONSUMO_REP_EST" possui o valor "S" e "CONSUMO_REP_EST_EMP" possui o valor "S". A Declaração de exportação deve possuir em seu conteúdo as flags "declarationItemExpoRepoStock" preenchida com o valor "S" e "declarationItemExpoRepoStockCompany" preenchida com o valor "S".&lt;/p&gt;</v>
+      </c>
+      <c r="D40" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;1 - Processo de exportação cadastrado (Exportação tipo 10 com CTIT)﻿ e com consumo de DI's do tipo IC e Remitos de Parceiro com motivo "R";&lt;br /&gt;
+2 - Arquivo XML contendo informações de Declaração de Exportação para o processo descrito na pré-condição de número 1 com as tags "declarationItemExpoRepoStock" preenchida com o valor "S"; e "declarationItemExpoRepoStockCompany" preenchida com o valor "S";&lt;br /&gt;
+3 - Usuário do In-Out com permissão para execução da interface de entrada "Broker2Softway" do Export Sys;&lt;br /&gt;
+4 - Usuário do Export Sys com permissão para consulta de Declaração de Exportação;&lt;br /&gt;
+5 - Usuário do IT Sys com permissão para consulta de Declaração de Exportação&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" customFormat="false">
+      <c r="A41" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B41" s="0" t="str">
+        <v>Receber DE XML via interface B2S para processo de exportação com consumo Remitos do tipo R</v>
+      </c>
+      <c r="C41" s="0" t="str">
+        <v>&lt;p&gt;Receber uma declaração de exportação via interface XML Broker2Softway de modo que o processo de exportação cadastrado possua consumo somente de Remitos de Parceiro com motivo "R", e consequentemente as flags "CONSUMO_REP_EST" possui o valor "S" e "CONSUMO_REP_EST_EMP" possui o valor "N". A Declaração de exportação deve possuir em seu conteúdo as flags "declarationItemExpoRepoStock" preenchida com o valor "N" e "declarationItemExpoRepoStockCompany" preenchida com o valor "S".&lt;/p&gt;</v>
+      </c>
+      <c r="D41" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;1 - Processo de exportação cadastrado (Exportação tipo 10 com CTIT)﻿ e com consumo apenas de Remitos de Parceiro com motivo "R";&lt;br /&gt;
+2 - Arquivo XML contendo informações de Declaração de Exportação para o processo descrito na pré-condição de número 1 com as tags "declarationItemExpoRepoStock" preenchida com o valor "S"; e "declarationItemExpoRepoStockCompany" preenchida com o valor "N";&lt;br /&gt;
+3 - Usuário do In-Out com permissão para execução da interface de entrada "Broker2Softway" do Export Sys;&lt;br /&gt;
+4 - Usuário do Export Sys com permissão para consulta de Declaração de Exportação;&lt;br /&gt;
+5 - Usuário do IT Sys com permissão para consulta de Declaração de Exportação.&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" customFormat="false">
+      <c r="A42" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B42" s="0" t="str">
+        <v>Receber DE XML via interface B2S para processo de exportação  com divergências 001</v>
+      </c>
+      <c r="C42" s="0" t="str">
+        <v>&lt;p&gt;Receber uma declaração de exportação via interface XML Broker2Softway de modo que o processo de exportação cadastrado possua consumo de DI's do tipo IC e Remitos de Parceiro com motivo "R", e consequentemente as flags "CONSUMO_REP_EST" possui o valor "S" e "CONSUMO_REP_EST_EMP" possui o valor "S". A Declaração de exportação deve possuir em seu conteúdo as flags "declarationItemExpoRepoStock" preenchida com o valor "N" e "declarationItemExpoRepoStockCompany" preenchida com o valor "N". Após carregar a Declaração de Exportação, o sistema deve registrar um log da divergência entre a sugestão de exportação e a declaração de exportação.&lt;/p&gt;</v>
+      </c>
+      <c r="D42" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;1 - Processo de exportação cadastrado (Exportação tipo 10 com CTIT)﻿ e com consumo de DI's do tipo IC e Remitos de Parceiro com motivo "R";&lt;br /&gt;
+2 - Arquivo XML contendo informações de Declaração de Exportação para o processo descrito na pré-condição de número 1 com as tags "declarationItemExpoRepoStock" preenchida com o valor "N"; e "declarationItemExpoRepoStockCompany" preenchida com o valor "N";&lt;br /&gt;
+3 - Usuário do In-Out com permissão para execução da interface de entrada "Broker2Softway" do Export Sys;&lt;br /&gt;
+4 - Usuário do Export Sys com permissão para consulta de Declaração de Exportação;&lt;br /&gt;
+5 - Usuário do IT Sys com permissão para consulta de Declaração de Exportação&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" customFormat="false">
+      <c r="A43" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B43" s="0" t="str">
+        <v>Receber DE XML via interface B2S para processo de exportação  com divergências 002</v>
+      </c>
+      <c r="C43" s="0" t="str">
+        <v>&lt;p&gt;Receber uma declaração de exportação via interface XML Broker2Softway de modo que o processo de exportação cadastrado possua consumo de DI's do tipo IC e Remitos de Parceiro com motivo "R", e consequentemente as flags "CONSUMO_REP_EST" possui o valor "S" e "CONSUMO_REP_EST_EMP" possui o valor "S". A Declaração de exportação deve possuir em seu conteúdo as flags "declarationItemExpoRepoStock" preenchida com o valor "N" e "declarationItemExpoRepoStockCompany" preenchida com o valor "S". Após carregar a Declaração de Exportação, o sistema deve registrar um log da divergência entre a sugestão de exportação e a declaração de exportação.&lt;/p&gt;</v>
+      </c>
+      <c r="D43" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;1 - Processo de exportação cadastrado (Exportação tipo 10 com CTIT)﻿ e com consumo de DI's do tipo IC e Remitos de Parceiro com motivo "R";&lt;br /&gt;
+2 - Arquivo XML contendo informações de Declaração de Exportação para o processo descrito na pré-condição de número 1 com as tags "declarationItemExpoRepoStock" preenchida com o valor "N"; e "declarationItemExpoRepoStockCompany" preenchida com o valor "S";&lt;br /&gt;
+3 - Usuário do In-Out com permissão para execução da interface de entrada "Broker2Softway" do Export Sys;&lt;br /&gt;
+4 - Usuário do Export Sys com permissão para consulta de Declaração de Exportação;&lt;br /&gt;
+5 - Usuário do IT Sys com permissão para consulta de Declaração de Exportação&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" customFormat="false">
+      <c r="A44" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B44" s="0" t="str">
+        <v>Receber DE XML via interface B2S para processo de exportação  com divergências 003</v>
+      </c>
+      <c r="C44" s="0" t="str">
+        <v>&lt;p&gt;Receber uma declaração de exportação via interface XML Broker2Softway de modo que o processo de exportação cadastrado possua consumo de DI's do tipo IC e Remitos de Parceiro com motivo "R", e consequentemente as flags "CONSUMO_REP_EST" possui o valor "S" e "CONSUMO_REP_EST_EMP" possui o valor "S". A Declaração de exportação deve possuir em seu conteúdo as flags "declarationItemExpoRepoStock" preenchida com o valor "S" e "declarationItemExpoRepoStockCompany" preenchida com o valor "N". Após carregar a Declaração de Exportação, o sistema deve registrar um log da divergência entre a sugestão de exportação e a declaração de exportação.&lt;/p&gt;</v>
+      </c>
+      <c r="D44" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;1 - Processo de exportação cadastrado (Exportação tipo 10 com CTIT)﻿ e com consumo de DI's do tipo IC e Remitos de Parceiro com motivo "R";&lt;br /&gt;
+2 - Arquivo XML contendo informações de Declaração de Exportação para o processo descrito na pré-condição de número 1 com as tags "declarationItemExpoRepoStock" preenchida com o valor "S"; e "declarationItemExpoRepoStockCompany" preenchida com o valor "N";&lt;br /&gt;
+3 - Usuário do In-Out com permissão para execução da interface de entrada "Broker2Softway" do Export Sys;&lt;br /&gt;
+4 - Usuário do Export Sys com permissão para consulta de Declaração de Exportação;&lt;br /&gt;
+5 - Usuário do IT Sys com permissão para consulta de Declaração de Exportação&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" customFormat="false">
+      <c r="A45" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B45" s="0" t="str">
+        <v>Receber DE XML via interface B2S para processo de exportação  com divergências 004</v>
+      </c>
+      <c r="C45" s="0" t="str">
+        <v>&lt;p&gt;Receber uma declaração de exportação via interface XML Broker2Softway de modo que o processo de exportação cadastrado possua consumo de DI's do tipo IC e Remitos de Parceiro com motivo "R", e consequentemente as flags "CONSUMO_REP_EST" possui o valor "S" e "CONSUMO_REP_EST_EMP" possui o valor "S". A Declaração de exportação deve possuir em seu conteúdo as flags "declarationItemExpoRepoStock" preenchida com o valor ""(Sem Preenchimento) e "declarationItemExpoRepoStockCompany" preenchida com o valor ""(Sem Preenchimento). Após carregar a Declaração de Exportação, o sistema deve registrar um log da divergência entre a sugestão de exportação e a declaração de exportação.&lt;/p&gt;</v>
+      </c>
+      <c r="D45" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;1 - Processo de exportação cadastrado (Exportação tipo 10 com CTIT)﻿ e com consumo de DI's do tipo IC e Remitos de Parceiro com motivo "R";&lt;br /&gt;
+2 - Arquivo XML contendo informações de Declaração de Exportação para o processo descrito na pré-condição de número 1 com as tags "declarationItemExpoRepoStock" preenchida com o valor ""(Sem Preenchimento); e "declarationItemExpoRepoStockCompany" preenchida com o valor ""(Sem Preenchimento);&lt;br /&gt;
+3 - Usuário do In-Out com permissão para execução da interface de entrada "Broker2Softway" do Export Sys;&lt;br /&gt;
+4 - Usuário do Export Sys com permissão para consulta de Declaração de Exportação;&lt;br /&gt;
+5 - Usuário do IT Sys com permissão para consulta de Declaração de Exportação&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" customFormat="false">
+      <c r="A46" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B46" s="0" t="str">
+        <v>Receber DE XML via interface B2S com alteração de DE já cadastrada  com divergências 001</v>
+      </c>
+      <c r="C46" s="0" t="str">
+        <v>&lt;p&gt;Receber uma declaração de exportação via interface XML Broker2Softway de modo que o processo de exportação cadastrado já com sua respectiva Declaração de Exportação possua consumo de DI's do tipo IC e Remitos de Parceiro com motivo "R", e consequentemente as flags "CONSUMO_REP_EST" possui o valor "S" e "CONSUMO_REP_EST_EMP" possui o valor "S". A Declaração de exportação deve possuir em seu conteúdo as flags "declarationItemExpoRepoStock" preenchida com o valor "N" e "declarationItemExpoRepoStockCompany" preenchida com o valor "N". Após carregar a Declaração de Exportação, o sistema deve registrar um log da divergência entre a sugestão de exportação e a declaração de exportação.&lt;/p&gt;</v>
+      </c>
+      <c r="D46" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;1 - Processo de exportação cadastrado (Exportação tipo 10 com CTIT)﻿ e com consumo de DI's do tipo IC e Remitos de Parceiro com motivo "R" com DE já cadastrada e enviada ao RegInt com as flags "CONSUMO_REP_EST"= "S" e "CONSUMO_REP_EST_EMP"="S";&lt;br /&gt;
+2 - Arquivo XML contendo informações de Declaração de Exportação para o processo descrito na pré-condição de número 1 com as tags "declarationItemExpoRepoStock" preenchida com o valor "N"; e "declarationItemExpoRepoStockCompany" preenchida com o valor "N";&lt;br /&gt;
+3 - Usuário do In-Out com permissão para execução da interface de entrada "Broker2Softway" do Export Sys;&lt;br /&gt;
+4 - Usuário do Export Sys com permissão para consulta de Declaração de Exportação;&lt;br /&gt;
+5 - Usuário do IT Sys com permissão para consulta de Declaração de Exportação&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" customFormat="false">
+      <c r="A47" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B47" s="0" t="str">
+        <v>Receber DE XML via interface B2S com alteração de DE já cadastrada  com divergências 002</v>
+      </c>
+      <c r="C47" s="0" t="str">
+        <v>&lt;p&gt;Receber uma declaração de exportação via interface XML Broker2Softway de modo que o processo de exportação cadastrado já com sua respectiva Declaração de Exportação possua consumo de DI's do tipo IC e Remitos de Parceiro com motivo "R", e consequentemente as flags "CONSUMO_REP_EST" possui o valor "S" e "CONSUMO_REP_EST_EMP" possui o valor "S". A Declaração de exportação deve possuir em seu conteúdo as flags "declarationItemExpoRepoStock" preenchida com o valor "N" e "declarationItemExpoRepoStockCompany" preenchida com o valor "S". Após carregar a Declaração de Exportação, o sistema deve registrar um log da divergência entre a sugestão de exportação e a declaração de exportação.&lt;/p&gt;</v>
+      </c>
+      <c r="D47" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;1 - Processo de exportação cadastrado (Exportação tipo 10 com CTIT)﻿ e com consumo de DI's do tipo IC e Remitos de Parceiro com motivo "R" com DE já cadastrada e enviada ao RegInt com as flags "CONSUMO_REP_EST"= "S" e "CONSUMO_REP_EST_EMP"="S";&lt;br /&gt;
+2 - Arquivo XML contendo informações de Declaração de Exportação para o processo descrito na pré-condição de número 1 com as tags "declarationItemExpoRepoStock" preenchida com o valor "N"; e "declarationItemExpoRepoStockCompany" preenchida com o valor "S";&lt;br /&gt;
+3 - Usuário do In-Out com permissão para execução da interface de entrada "Broker2Softway" do Export Sys;&lt;br /&gt;
+4 - Usuário do Export Sys com permissão para consulta de Declaração de Exportação;&lt;br /&gt;
+5 - Usuário do IT Sys com permissão para consulta de Declaração de Exportação&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" customFormat="false">
+      <c r="A48" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B48" s="0" t="str">
+        <v>Receber DE XML via interface B2S com alteração de DE já cadastrada  com divergências 003</v>
+      </c>
+      <c r="C48" s="0" t="str">
+        <v>&lt;p&gt;Receber uma declaração de exportação via interface XML Broker2Softway de modo que o processo de exportação cadastrado já com sua respectiva Declaração de Exportação possua consumo de DI's do tipo IC e Remitos de Parceiro com motivo "R", e consequentemente as flags "CONSUMO_REP_EST" possui o valor "S" e "CONSUMO_REP_EST_EMP" possui o valor "S". A Declaração de exportação deve possuir em seu conteúdo as flags "declarationItemExpoRepoStock" preenchida com o valor "S" e "declarationItemExpoRepoStockCompany" preenchida com o valor "N". Após carregar a Declaração de Exportação, o sistema deve registrar um log da divergência entre a sugestão de exportação e a declaração de exportação.&lt;/p&gt;</v>
+      </c>
+      <c r="D48" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;1 - Processo de exportação cadastrado (Exportação tipo 10 com CTIT)﻿ e com consumo de DI's do tipo IC e Remitos de Parceiro com motivo "R" com DE já cadastrada e enviada ao RegInt com as flags "CONSUMO_REP_EST"= "S" e "CONSUMO_REP_EST_EMP"="S";&lt;br /&gt;
+2 - Arquivo XML contendo informações de Declaração de Exportação para o processo descrito na pré-condição de número 1 com as tags "declarationItemExpoRepoStock" preenchida com o valor "S"; e "declarationItemExpoRepoStockCompany" preenchida com o valor "N";&lt;br /&gt;
+3 - Usuário do In-Out com permissão para execução da interface de entrada "Broker2Softway" do Export Sys;&lt;br /&gt;
+4 - Usuário do Export Sys com permissão para consulta de Declaração de Exportação;&lt;br /&gt;
+5 - Usuário do IT Sys com permissão para consulta de Declaração de Exportação&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" customFormat="false">
+      <c r="A49" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B49" s="0" t="str">
+        <v>Integração Export Sys X IT Sys</v>
+      </c>
+      <c r="C49" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;Suite de testes para a funcionalidade Integração Export Sys X IT Sys.&lt;/p&gt; 
+</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" customFormat="false">
+      <c r="A50" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B50" s="0" t="str">
+        <v>Entidades</v>
+      </c>
+      <c r="C50" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt; Suíte com testes das entidades do sistema.&lt;/p&gt; 
+</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" customFormat="false">
+      <c r="A51" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B51" s="0" t="str">
+        <v>Cadastrar um Sistema Externo</v>
+      </c>
+      <c r="C51" s="0" t="str">
+        <v>&lt;p&gt;Verificar o cadastro de um novo Sistema Externo através do IT Sys.&lt;/p&gt;</v>
+      </c>
+      <c r="D51" s="0" t="str">
+        <v>&lt;p&gt;1 - Usuário do IT Sys com permissão de acesso ao cadastro de Sistemas Externos.&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" customFormat="false">
+      <c r="A52" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B52" s="0" t="str">
+        <v>Alterar um Sistema Externo</v>
+      </c>
+      <c r="C52" s="0" t="str">
+        <v>&lt;p&gt;Verificar a alteração de um Sistema Externo através do IT Sys.&lt;/p&gt;</v>
+      </c>
+      <c r="D52" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;1 - Usuário do IT Sys com permissão de acesso ao cadastro de Sistemas Externos;&lt;br /&gt;
+2 - Sistema Externo cadastrado.&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" customFormat="false">
+      <c r="A53" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B53" s="0" t="str">
+        <v>Excluir um Sistema Externo</v>
+      </c>
+      <c r="C53" s="0" t="str">
+        <v>&lt;p&gt;Verificar a Exclusão de um Sistema Externo através do IT Sys.&lt;/p&gt;</v>
+      </c>
+      <c r="D53" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;1 - Usuário do IT Sys com permissão de acesso ao cadastro de Sistemas Externos;&lt;br /&gt;
+2 - Sistema Externo cadastrado, não utilizado em outros pontos do Sistema.&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" customFormat="false">
+      <c r="A54" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B54" s="0" t="str">
+        <v>Exclusão de Sistema não ocorre por quebra de regras de validação</v>
+      </c>
+      <c r="C54" s="0" t="str">
+        <v>&lt;p&gt;Verificar que o Sistema não permite a exclusão de um Sistema Externo quando o mesmo está em utilização em outros pontos do Sistema.&lt;/p&gt;</v>
+      </c>
+      <c r="D54" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;1 - Usuário do IT Sys com permissão de acesso ao cadastro de Sistemas Externos;&lt;br /&gt;
+2 - Sistema Externo cadastrado, utilizado em outros pontos do Sistema.&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" customFormat="false">
+      <c r="A55" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B55" s="0" t="str">
+        <v>Cadastro de Sistema Externo, não ocorre por quebra de regras de validação</v>
+      </c>
+      <c r="C55" s="0" t="str">
+        <v>&lt;p&gt;Verificar o cadastro de um novo Sistema Externo através do IT Sys.&lt;/p&gt;</v>
+      </c>
+      <c r="D55" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;1 - Usuário do IT Sys com permissão de acesso ao cadastro de Sistemas Externos;&lt;br /&gt;
+2 - Sistema Externo cadastrado.&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" customFormat="false">
+      <c r="A56" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B56" s="0" t="str">
+        <v>Verificar Filtro de associação de sistemas internos e sistemas externos</v>
+      </c>
+      <c r="C56" s="0" t="str">
+        <v>&lt;p&gt;Verificar o filtro de busca de Associação de Sistemas Internos&lt;/p&gt;</v>
+      </c>
+      <c r="D56" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;1 - Usuário do IT Sys com permissão de acesso ao vínculo de Sistemas Internos e Sistemas Externos;&lt;br /&gt;
+2 - Sistemas Internos cadastrados no sistema;&lt;br /&gt;
+3 - Sistemas Externos cadastrados no sistema;&lt;br /&gt;
+4 - Vinculos entre Sistemas Internos e Sistemas Externos cadastrados.&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" customFormat="false">
+      <c r="A57" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B57" s="0" t="str">
+        <v>Cadastrar vínculo entre Sistema Interno e Sistema Externo</v>
+      </c>
+      <c r="C57" s="0" t="str">
+        <v>&lt;p&gt;Verificar o cadastro de um vínculo entre Sistema Interno e Sistema Externos.&lt;/p&gt;</v>
+      </c>
+      <c r="D57" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;1 - Usuário do IT Sys com permissão de acesso ao vínculo de Sistemas Internos e Sistemas Externos;&lt;br /&gt;
+2 - Sistemas Internos cadastrados no sistema;&lt;br /&gt;
+3 - Sistemas Externos cadastrados no sistema.&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" customFormat="false">
+      <c r="A58" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B58" s="0" t="str">
+        <v>Alterar vínculo entre Sistema Interno e Sistema Externo</v>
+      </c>
+      <c r="C58" s="0" t="str">
+        <v>&lt;p&gt;Verificar a operação de alteração de um vínculo entre Sistema Interno e Sistema Externos já cadastrado.&lt;/p&gt;</v>
+      </c>
+      <c r="D58" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;1 - Usuário do IT Sys com permissão de acesso ao vínculo de Sistemas Internos e Sistemas Externos;&lt;br /&gt;
+2 - Sistemas Internos cadastrados no sistema;&lt;br /&gt;
+3 - Sistemas Externos cadastrados no sistema;&lt;br /&gt;
+4 - Vínculo entre Sistema Interno e Sistema Externo cadastrado.&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" customFormat="false">
+      <c r="A59" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B59" s="0" t="str">
+        <v>Excluir vínculo entre Sistema Interno e Sistema Externo</v>
+      </c>
+      <c r="C59" s="0" t="str">
+        <v>&lt;p&gt;Verificar a operação de exclusão de um vínculo entre Sistema Interno e Sistema Externo já cadastrado.&lt;/p&gt;</v>
+      </c>
+      <c r="D59" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;1 - Usuário do IT Sys com permissão de acesso ao vínculo de Sistemas Internos e Sistemas Externos;&lt;br /&gt;
+2 - Vínculo entre Sistema Interno e Sistema Externo cadastrado.&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" customFormat="false">
+      <c r="A60" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B60" s="0" t="str">
+        <v>Cadastro de vínculo entre Sistema Interno e Sistema Externo não ocorre por erros de validação</v>
+      </c>
+      <c r="C60" s="0" t="str">
+        <v>&lt;p&gt;Verificar que um cadastro de vínculo entre Sistema Interno e Sistema Externo não ocorre devido a quebra de regras de validação.&lt;/p&gt;</v>
+      </c>
+      <c r="D60" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;1 - Usuário do IT Sys com permissão de acesso ao vínculo de Sistemas Internos e Sistemas Externos;&lt;br /&gt;
+2 - Vínculo de Sistema Interno com Sistema Externo Cadastrado.&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" customFormat="false">
+      <c r="A61" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B61" s="0" t="str">
+        <v>Validação dos Filtros</v>
+      </c>
+      <c r="C61" s="0" t="str">
+        <v/>
+      </c>
+      <c r="D61" s="0" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="1:4" customFormat="false">
+      <c r="A62" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B62" s="0" t="str">
+        <v>Cadastro de Família</v>
+      </c>
+      <c r="C62" s="0" t="str">
+        <v/>
+      </c>
+      <c r="D62" s="0" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="1:4" customFormat="false">
+      <c r="A63" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B63" s="0" t="str">
+        <v>Cadastro de OP Estática</v>
+      </c>
+      <c r="C63" s="0" t="str">
+        <v>&lt;p&gt;Gerar OP estática.&lt;/p&gt;</v>
+      </c>
+      <c r="D63" s="0" t="str">
+        <v>&lt;p&gt; Ter produtos acabado e insumos para serem vinculados na OP.&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" customFormat="false">
+      <c r="A64" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B64" s="0" t="str">
+        <v>Validação Aba Pedidos</v>
+      </c>
+      <c r="C64" s="0" t="str">
+        <v>&lt;p&gt; Validação dos campos e regras do cadastro de CTIT&lt;/p&gt;</v>
+      </c>
+      <c r="D64" s="0" t="str">
+        <v>&lt;p&gt;Ter OP cadastrada&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" customFormat="false">
+      <c r="A65" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B65" s="0" t="str">
+        <v>Validação Aba Importações e Exportações - Inclusão do Acabado</v>
+      </c>
+      <c r="C65" s="0" t="str">
+        <v>&lt;p&gt; Validação dos campos e regras do cadastro de Importações e Exportações&lt;/p&gt;</v>
+      </c>
+      <c r="D65" s="0" t="str">
+        <v>&lt;p&gt;Ter CTIT com dados da capa cadastrado&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" customFormat="false">
+      <c r="A66" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B66" s="0" t="str">
+        <v>Validação Aba Importações e Exportações - Inclusão dos Componentes</v>
+      </c>
+      <c r="C66" s="0" t="str">
+        <v>&lt;p&gt; Validação dos campos e regras do cadastro de Importações e Exportações&lt;/p&gt;</v>
+      </c>
+      <c r="D66" s="0" t="str">
+        <v>&lt;p&gt;Ter CTIT com dados da capa cadastrado&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" customFormat="false">
+      <c r="A67" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B67" s="0" t="str">
+        <v>Validação Aba Inspeção e Responsável</v>
+      </c>
+      <c r="C67" s="0" t="str">
+        <v/>
+      </c>
+      <c r="D67" s="0" t="str">
+        <v>&lt;p&gt;Ter CTIT com dados da capa cadastrado&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" customFormat="false">
+      <c r="A68" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B68" s="0" t="str">
+        <v>Validação Aba Retificação</v>
+      </c>
+      <c r="C68" s="0" t="str">
+        <v/>
+      </c>
+      <c r="D68" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;- Ter um CTIT cadastrado e aprovado.&lt;br /&gt;
+- Ter uma retificação cadastrada para o CTIT (caso contrário o único dado preenchido será no campo de Referência).&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" customFormat="false">
+      <c r="A69" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B69" s="0" t="str">
+        <v>Cadastro de CTIT com Familia</v>
+      </c>
+      <c r="C69" s="0" t="str">
+        <v>&lt;p&gt; Testes de inclusão e alteração de CTIT com familia ativa/inativa.&lt;/p&gt;</v>
+      </c>
+      <c r="D69" s="0" t="str">
+        <v>&lt;p&gt; Tem familia cadastrada&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" customFormat="false">
+      <c r="A70" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B70" s="0" t="str">
+        <v>Filtro do Cadastro de Previsão de Exportação</v>
+      </c>
+      <c r="C70" s="0" t="str">
+        <v>&lt;p&gt;Manipular os campos de filtro do cadastro de Previsão de Exportação.&lt;/p&gt;</v>
+      </c>
+      <c r="D70" s="0" t="str">
+        <v>&lt;p&gt;Ter Previsões cadastradas para testes de filtro&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" customFormat="false">
+      <c r="A71" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B71" s="0" t="str">
+        <v>Cadastro de Previsão de Exportação - Capa</v>
+      </c>
+      <c r="C71" s="0" t="str">
+        <v>&lt;p&gt;Cadastro da Previsão de Exportação dados de Capa.&lt;/p&gt;</v>
+      </c>
+      <c r="D71" s="0" t="str">
+        <v>&lt;p&gt;&lt;span style="font-family: Calibri, sans-serif; font-size: 13.3333px; line-height: 15.3333px;"&gt;Para determinar o uso de forecast é preciso ativar o parâmetro CTRL_FORECAST_VL_EXP = S.&lt;/span&gt;&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" customFormat="false">
+      <c r="A72" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B72" s="0" t="str">
+        <v>Previsão de Exportação Aba Importação Temporal</v>
+      </c>
+      <c r="C72" s="0" t="str">
+        <v>&lt;p&gt;Cadastro da Previsão de Exportação para Importação Temporal = IT&lt;/p&gt;</v>
+      </c>
+      <c r="D72" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;&lt;font face="Calibri, sans-serif"&gt;&lt;span style="font-size: 13.3333px; line-height: 15.3333px;"&gt;Ter preenchido os dados de capa da previsão conforme descrito no CT 443: Cadastro de &lt;/span&gt;&lt;/font&gt;Previsão de Exportação - Capa.&lt;/p&gt;
+&lt;p&gt;Configurar o Regime Aduaneiro no menu: Cadastros &gt; Configuração de Regime Aduaneiro e para o parâmetro IMPORTACAO_TEMPORAL no campo "Utiliza Previsão" deixar = SIM.&lt;/p&gt;
+&lt;p&gt; &lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" customFormat="false">
+      <c r="A73" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B73" s="0" t="str">
+        <v>Previsão de Exportação Aba Automotriz</v>
+      </c>
+      <c r="C73" s="0" t="str">
+        <v>&lt;p&gt; Cadastro da Previsão de Exportação para Importação Automotiva = IA&lt;/p&gt;</v>
+      </c>
+      <c r="D73" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;&lt;span style="font-family: Calibri, sans-serif; font-size: 13.3333px; line-height: 15.3333px;"&gt;Para determinar o uso de forecast é preciso ativar o parâmetro CTRL_FORECAST_VL_EXP = S.&lt;/span&gt;&lt;/p&gt;
+&lt;p&gt;No Import Sys, inserir a classificação fiscal dos insumos no menu: Configurações &gt; Regime Aduaneiro, para o regime normal integral. Botão Vincular Classif. Fiscal.&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" customFormat="false">
+      <c r="A74" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B74" s="0" t="str">
+        <v>Previsão de Exportação Aba Consumo</v>
+      </c>
+      <c r="C74" s="0" t="str">
+        <v>&lt;p&gt; Cadastro da Previsão de Exportação para Importação a Consumo = IC&lt;/p&gt;</v>
+      </c>
+      <c r="D74" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;&lt;span style="font-family: Calibri, sans-serif; font-size: 10pt; line-height: 115%;"&gt;Para determinar o uso de forecast é preciso ativar o parâmetro CTRL_FORECAST_VL_EXP = S.&lt;/span&gt;&lt;/p&gt;
+&lt;p&gt;Configurar o Regime Aduaneiro no menu: Cadastros &gt; Configuração de Regime Aduaneiro e para o parâmetro CONSUMO no campo "Utiliza Previsão" deixar = SIM.&lt;/p&gt;
+&lt;p&gt; &lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" customFormat="false">
+      <c r="A75" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B75" s="0" t="str">
+        <v>Forecast para Importação com Família</v>
+      </c>
+      <c r="C75" s="0" t="str">
+        <v>&lt;p&gt;Validar se sistema utiliza famólia ativa para realizar ou não forecast.&lt;/p&gt;</v>
+      </c>
+      <c r="D75" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;Ter executado os testes de Configurações para Forecast&lt;/p&gt;
+&lt;p&gt;Ter produto com família ativa cadastrada e o produto ativo na família.&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" customFormat="false">
+      <c r="A76" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B76" s="0" t="str">
+        <v>Validar Forecast - OP com Perda Tangível</v>
+      </c>
+      <c r="C76" s="0" t="str">
+        <v>&lt;p&gt;Verificar se o forecast esta sendo realizado corretamente quando a op esta sem quantidade de perda tangível para os insumos.&lt;/p&gt;</v>
+      </c>
+      <c r="D76" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;- Produto acabado deve ter OP e seus insumos devem ter quantidades de perdas tangíveis.&lt;/p&gt;
+&lt;p&gt;- Ter o CTIT gerado e válido para o Produto.&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" customFormat="false">
+      <c r="A77" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B77" s="0" t="str">
+        <v>Validar Forecast - Via Interface</v>
+      </c>
+      <c r="C77" s="0" t="str">
+        <v>&lt;p&gt;Verificar se o forecast esta sendo realizado corretamente quando o produto está dentro de uma família ativa/inativa. &lt;/p&gt;</v>
+      </c>
+      <c r="D77" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt;- Produto acabado deve ter OP e seus insumos deve estar com quantidades de perdas preenchidas.&lt;/p&gt;
+&lt;p&gt;- Produto acabado deve pertencer a uma família ativa.&lt;/p&gt;
+&lt;p&gt;- Ter planilha de apontamento manual em anexo a esse CT.&lt;/p&gt;
+&lt;p&gt;- Interface configurada para maquina do usuário no inout.&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" customFormat="false">
+      <c r="A78" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B78" s="0" t="str">
+        <v>Exclusão de DI</v>
+      </c>
+      <c r="C78" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt; Validar a exclusão da DI para os seguintes cenários:&lt;/p&gt;
+&lt;p&gt;&lt;b style="text-align: justify;"&gt;           DI com consumo antecipado de MRSP&lt;/b&gt;&lt;/p&gt;
+&lt;p class="MsoNormal" style="text-align:justify;text-justify:inter-ideograph"&gt;&lt;b&gt;            DI com baixa&lt;o:p&gt;&lt;/o:p&gt;&lt;/b&gt;&lt;/p&gt;
+&lt;p class="MsoNormal" style="text-align:justify;text-justify:inter-ideograph"&gt;&lt;b&gt;            DI sem baixa e sem consumo de MRSP&lt;o:p&gt;&lt;/o:p&gt;&lt;/b&gt;&lt;/p&gt;
+&lt;p class="MsoNormal" style="text-align:justify;text-justify:inter-ideograph"&gt;&lt;b&gt;            DI com saldo suspenso&lt;o:p&gt;&lt;/o:p&gt;&lt;/b&gt;&lt;/p&gt;
+&lt;p class="MsoNormal" style="text-align:justify;text-justify:inter-ideograph"&gt;&lt;b&gt;            DI nacionalizada&lt;o:p&gt;&lt;/o:p&gt;&lt;/b&gt;&lt;/p&gt;
+&lt;p&gt; &lt;/p&gt;</v>
+      </c>
+      <c r="D78" s="0" t="str">
+        <v>&lt;p&gt; Ter DIs cadastradas no Import Sys&lt;/p&gt;</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" customFormat="false">
+      <c r="A79" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B79" s="0" t="str">
+        <v>Cadastro de Sistemas</v>
+      </c>
+      <c r="C79" s="0" t="str">
+        <v xml:space="preserve"> 
+</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" customFormat="false">
+      <c r="A80" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B80" s="0" t="str">
+        <v>Família</v>
+      </c>
+      <c r="C80" s="0" t="str">
+        <v xml:space="preserve">&lt;div&gt;A família serve para que a empresa cadastre um produto acabado “genérico”, e para este produto teremos outros produtos acabados vinculado a ele, exemplo:&lt;/div&gt;
+&lt;div&gt; &lt;/div&gt;
+&lt;div&gt;FAMÍLIA: GOL&lt;/div&gt;
+&lt;div&gt; &lt;/div&gt;
+&lt;div&gt;PRODUTOS QUE PERTENCEM A FAMÍLIA GOL:&lt;/div&gt;
+&lt;div&gt;•&lt;span class="Apple-tab-span" style="white-space:pre"&gt;	&lt;/span&gt;GOL 1.0 8V GL&lt;/div&gt;
+&lt;div&gt;•&lt;span class="Apple-tab-span" style="white-space:pre"&gt;	&lt;/span&gt;GOL 1.0 16V GL&lt;/div&gt;
+&lt;div&gt;•&lt;span class="Apple-tab-span" style="white-space:pre"&gt;	&lt;/span&gt;GOL 1.6 8V GTI&lt;/div&gt;
+&lt;div&gt;•&lt;span class="Apple-tab-span" style="white-space:pre"&gt;	&lt;/span&gt;GOL 2.0 8V GTI&lt;/div&gt;
+&lt;div&gt; &lt;/div&gt;
+&lt;div&gt;As empresas precisam informar ao governo, quais componentes/insumos eles terão que importar, e para que serão utilizados os componentes importados. Como não há como ter uma previsão correta de qual produto será produzido com o insumo importado, já que pode ser utilizado em mais de um produto acabado, a empresa informa que a importação será utilizada para produzir “GOL” e que na família GOL temos várias variedades.&lt;/div&gt; 
+</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" customFormat="false">
+      <c r="A81" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B81" s="0" t="str">
+        <v>OP - Ordem de Produção</v>
+      </c>
+      <c r="C81" s="0" t="str">
+        <v xml:space="preserve">&lt;div&gt;O apontamento de Ordem de Produção/ Árvore de Produto é o que define a composição da estrutura do produto acabado a ser exportado, considerando os insumos e quantidades utilizadas em sua produção e o tempo demandado para isso.&lt;/div&gt;
+&lt;p&gt; &lt;/p&gt; 
+</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" customFormat="false">
+      <c r="A82" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B82" s="0" t="str">
+        <v>CTIT</v>
+      </c>
+      <c r="C82" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt; Casos de testes do cadastro de CTIT&lt;/p&gt; 
+</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" customFormat="false">
+      <c r="A83" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B83" s="0" t="str">
+        <v>Previsão de Exportação - Forecast</v>
+      </c>
+      <c r="C83" s="0" t="str">
+        <v xml:space="preserve">&lt;p class="MsoNormal" style="margin-bottom: 0.0001pt;"&gt;&lt;b&gt;&lt;span style="font-size:10.0pt;font-family:"Calibri,Bold","sans-serif";mso-bidi-font-family:
+"Calibri\,Bold""&gt;Forecast &lt;/span&gt;&lt;/b&gt;&lt;span style="font-size:10.0pt;mso-ascii-font-family:
+Calibri;mso-hansi-font-family:Calibri;mso-bidi-font-family:Calibri"&gt;– Projeção de importação, vendas locais, exportação e de produção, ou ainda planejamento de setores como compras, financeiro, custos - muito utilizado em processos de logística.&lt;/span&gt;&lt;/p&gt;
+&lt;p class="MsoNormal" style="margin-bottom: 0.0001pt;"&gt;&lt;span style="font-size: 10pt;"&gt;A utilização de forecast é indicada para empresas cujos produtos acabados têm parte de seu saldo exportado e outra parte vendida no mercado nacional, pois apenas a parte dos insumos que foi exportada pode ser beneficiada pelo uso do regime de Importação Temporal.&lt;/span&gt;&lt;/p&gt;
+&lt;p class="MsoNormal" style="margin-bottom: 0.0001pt;"&gt;&lt;span style="font-size:
+10.0pt;mso-ascii-font-family:Calibri;mso-hansi-font-family:Calibri;mso-bidi-font-family:
+Calibri"&gt;&lt;o:p&gt;&lt;/o:p&gt;&lt;/span&gt;&lt;/p&gt;
+&lt;p class="MsoNormal" style="margin-bottom: 0.0001pt;"&gt;&lt;span style="font-size: 10pt;"&gt; &lt;/span&gt;&lt;span style="font-size:10.0pt;mso-ascii-font-family:
+Calibri;mso-hansi-font-family:Calibri;mso-bidi-font-family:Calibri"&gt;&lt;o:p&gt;&lt;/o:p&gt;&lt;/span&gt;&lt;/p&gt; 
+</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" customFormat="false">
+      <c r="A84" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B84" s="0" t="str">
+        <v>Declaração de Importação - DI</v>
+      </c>
+      <c r="C84" s="0" t="str">
+        <v xml:space="preserve">&lt;p&gt; Tratamento na exclusão da DI quando a mesma possui ou não integração e baixa no RegInt&lt;/p&gt; 
+</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" customFormat="false">
+      <c r="A85" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B85" s="0" t="str">
+        <v>Funcionalidades</v>
+      </c>
+      <c r="C85" s="0" t="str">
+        <v xml:space="preserve"> 
+</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" customFormat="false">
+      <c r="A86" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B86" s="0" t="str">
+        <v xml:space="preserve">Verificar funcionalidades disponíveis para o módulo </v>
+      </c>
+      <c r="C86" s="0" t="str">
+        <v/>
+      </c>
+      <c r="D86" s="0" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="1:3" customFormat="false">
+      <c r="A87" s="0" t="str">
+        <v>Argentina - RegInt Sys</v>
+      </c>
+      <c r="B87" s="0" t="str">
+        <v>Controle de Módulos</v>
+      </c>
+      <c r="C87" s="0" t="str">
+        <v xml:space="preserve"> 
+</v>
+      </c>
+    </row>
+  </sheetData>
 </worksheet>
 </file>
</xml_diff>